<commit_message>
Day_1 | Final Commit
</commit_message>
<xml_diff>
--- a/Batch/14/In_Class/Day_1.xlsx
+++ b/Batch/14/In_Class/Day_1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\14\In_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A8EC01-5373-456B-BA0F-92B5CE5AEEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AF608B-1641-4092-ACD4-E1A2E2884E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="750" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="750" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro_to_Data_Science" sheetId="3" r:id="rId1"/>
     <sheet name="Guidelines" sheetId="2" r:id="rId2"/>
     <sheet name="Intro_To_Excel" sheetId="1" r:id="rId3"/>
+    <sheet name="Introduction_Soft Skill" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="402">
   <si>
     <t>Why Data Science</t>
   </si>
@@ -3173,6 +3174,75 @@
   </si>
   <si>
     <t>If Yes how If No Why</t>
+  </si>
+  <si>
+    <t>Arpit Verma</t>
+  </si>
+  <si>
+    <t>Muthu Ram</t>
+  </si>
+  <si>
+    <t>Bhajneet Kaur</t>
+  </si>
+  <si>
+    <t>Arshul Khan</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>Ankit</t>
+  </si>
+  <si>
+    <t>Vikas</t>
+  </si>
+  <si>
+    <t>Murali</t>
+  </si>
+  <si>
+    <t>Anand</t>
+  </si>
+  <si>
+    <t>Gurumoorthy</t>
+  </si>
+  <si>
+    <t>Abina</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Subedar</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Academics</t>
+  </si>
+  <si>
+    <t>Work Exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skills </t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Goal</t>
   </si>
 </sst>
 </file>
@@ -3284,9 +3354,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3302,15 +3369,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3321,6 +3379,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3813,8 +3883,8 @@
       <xdr:row>138</xdr:row>
       <xdr:rowOff>85402</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="50" name="Ink 49">
@@ -3833,7 +3903,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="50" name="Ink 49">
@@ -3966,8 +4036,8 @@
       <xdr:row>154</xdr:row>
       <xdr:rowOff>38254</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="72" name="Ink 71">
@@ -3986,7 +4056,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="72" name="Ink 71">
@@ -4207,8 +4277,8 @@
       <xdr:row>184</xdr:row>
       <xdr:rowOff>94025</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="80" name="Ink 79">
@@ -4227,7 +4297,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="80" name="Ink 79">
@@ -4272,8 +4342,8 @@
       <xdr:row>190</xdr:row>
       <xdr:rowOff>8278</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="89" name="Ink 88">
@@ -4292,7 +4362,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="89" name="Ink 88">
@@ -4337,8 +4407,8 @@
       <xdr:row>189</xdr:row>
       <xdr:rowOff>10669</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="93" name="Ink 92">
@@ -4357,7 +4427,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="93" name="Ink 92">
@@ -4402,8 +4472,8 @@
       <xdr:row>187</xdr:row>
       <xdr:rowOff>46341</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="117" name="Ink 116">
@@ -4422,7 +4492,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="117" name="Ink 116">
@@ -4467,8 +4537,8 @@
       <xdr:row>189</xdr:row>
       <xdr:rowOff>142707</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="118" name="Ink 117">
@@ -4487,7 +4557,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="118" name="Ink 117">
@@ -4532,8 +4602,8 @@
       <xdr:row>192</xdr:row>
       <xdr:rowOff>66018</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="122" name="Ink 121">
@@ -4552,7 +4622,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="122" name="Ink 121">
@@ -4597,8 +4667,8 @@
       <xdr:row>191</xdr:row>
       <xdr:rowOff>112074</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="126" name="Ink 125">
@@ -4617,7 +4687,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="126" name="Ink 125">
@@ -4742,7 +4812,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2835.18">170 3058 704,'0'0'4781,"22"-9"-3516,169-65 3489,-152 64-4048,0 1 1,1 2 0,44-3-1,124 4-222,-121 4-155,550-3 677,113-4-643,1001 23-281,-1311 19-98,111 2 78,-511-35-41,50 1 25,0-3 0,169-28 1,-257 30-44,8-2 13,-1 1 0,1-2 0,0 1 0,-1-2 0,1 1 0,-1-1 0,0-1 0,0 1-1,12-10 1,-20 13-57,-1 0-1,1 1 0,-1-1 0,0 0 1,1 1-1,-1-1 0,0 0 1,1 1-1,-1-1 0,0 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1 0 0,1 1 1,0-1-1,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 0 0,0 1 1,1 0-1,-1-1 0,0 1 0,1-1 1,-1 1-1,0 0 0,0-1 0,1 1 1,-3 0-1,-39-14-4976</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3811.04">1665 0 3185,'0'0'4808,"1"6"-4600,6 77 332,-2 1 0,-10 115-1,-36 120 700,15-158-898,-87 717 857,77-586-777,15 55-53,16-192-74,-4-62-107,-1 22-836,15-131-7378,0-12 3251</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4447.25">2700 31 2609,'0'0'4373,"0"5"-3896,-4 54 49,-2-1 0,-20 86 0,-1 5 17,-50 494 1142,-41 269-947,91-759-45,-51 371 521,76-383-1422,2-141 160,1-1 0,-1 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,0-1-1,0 1 1,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1 0,1-1 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,1 0 1,-1 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 1 0,12-16-2822,11-20-2127</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5067.47">3720 29 2081,'0'0'3599,"-2"14"-3316,-33 216 2590,-7 46-888,7 118-255,-50 331-392,52-559-1092,-98 597 661,130-677-1252,9-91-4161,12-14 1361,0-10-1500</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5067.46">3720 29 2081,'0'0'3599,"-2"14"-3316,-33 216 2590,-7 46-888,7 118-255,-50 331-392,52-559-1092,-98 597 661,130-677-1252,9-91-4161,12-14 1361,0-10-1500</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5684.26">4653 26 1985,'0'0'4981,"-1"10"-3367,-30 148-1162,9-56 11,-114 894 2645,26-253-787,94-654-1993,-2 51 325,-1 156 0,16-229-537,-15 84 191,18-151-451,0-20-3711,0-13-1443</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6651.03">374 642 448,'0'0'3861,"28"0"-2962,342 0 2428,324-12-1254,307-1-1193,20 38-811,-670-3-59,698 24 12,-961-47-68,0 5 0,89 15 0,-159-17 23,-14-2-43,-1 0-1,0 0 0,1 0 1,-1 1-1,0-1 1,1 1-1,-1 0 0,0 0 1,0 0-1,5 3 1</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7562.05">195 1194 2193,'0'0'5488,"26"0"-4442,450 14 3121,642 23-2190,-622-23-1932,957 81-290,-1270-75-71,261 17-510,-152-28 52,115 1 542,-405-10-101,-6-6-4312,-12-2-1203</inkml:trace>
@@ -4893,7 +4963,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7101.18">3658 1798 3426,'0'0'10095,"-21"17"-9375,-64 60-98,79-70-531,-1 1 0,1-1 0,1 1-1,-1 0 1,1 0 0,1 1 0,-1 0 0,1-1 0,1 1 0,-4 16 0,4-6 87,1-1 1,0 0 0,2 31-1,1-20-142,-1-27-39,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,3-2 0,2 1 17,0 0-1,-1 0 0,1-1 0,0 0 1,0 0-1,-1-1 0,1 1 1,7-6-1,-2-2 63,1-1 0,-1 0 0,-1-1-1,0 0 1,-1 0 0,0-1 0,-1 0 0,0-1 0,-1 0 0,-1 0 0,8-25 0,-8 17-62,-1 0 1,-1-1 0,0 0 0,-2 0 0,-1 0 0,-1 0 0,-3-26 0,2 46-15,0 0 1,0 0-1,0 0 1,-1 0 0,0 0-1,1 1 1,-1-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,-1 1 1,1 0 0,-1 0-1,1 0 1,-1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0 0 1,0 0 0,0 0-1,0 1 1,-1-1-1,1 1 1,0 0-1,-6 0 1,5-1-90,0 1 1,-1 0-1,1 0 0,-1 1 1,1 0-1,-1-1 0,1 1 1,0 1-1,-8 2 0,11-4-84,-1 1 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 1-1,1-1 1,0 0 0,-1 1-1,1-1 1,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1-1,1 0 1,-1 0 0,0 0-1,0 2 1,0 19-3629,1-4-1072</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7303.11">3671 1798 3602</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7913.5">3671 1785 3602,'137'11'1536,"-135"-10"-1407,1-1 0,0 0-1,-1 1 1,1-1 0,-1 1-1,1 0 1,0 0 0,-1 0-1,0 0 1,1 0 0,-1 1-1,0-1 1,3 3 0,2 14 834,-6-11-537,6 23 417,-1 1 0,-1-1 0,-2 1 0,-1 0 0,-3 45 0,1-30-421,-1-45-367,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,1 0 36,1 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1-1 0,0 1 0,-1-1 1,1 0-1,0 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,-1-2-1,0-5-85,0 0-1,1 0 1,0 0-1,0 0 1,1-1 0,-1 1-1,2 0 1,-1 0 0,1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0-1,0 1 1,0-1 0,1 1-1,0 0 1,1 0 0,-1 0-1,1 1 1,1-1 0,6-6-1,16-13-380,0 1 1,2 1-1,59-36 0,-44 30 88,-21 14 33,-1 0 0,-1-2 0,-1-1 0,26-28 0,-40 39 354,-1-1-1,1 0 1,-2 0 0,1 0 0,-1 0-1,-1-1 1,0 0 0,0 0 0,-1-1 0,0 1-1,0 0 1,-2-1 0,1 0 0,-1-14-1,-3 3 1150,2 22-1241,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 1,0-1-1,-13 38-129,11-30 120,-18 74 91,3 1-1,4 0 1,-2 100 0,15-182-53,8-6 184,5-12-33,8-12-64,2 0 1,1 2 0,29-26 0,-45 46-143,0 0-1,1 0 1,1 1 0,-1 0 0,1 1 0,0 0-1,0 0 1,0 1 0,0 1 0,1 0 0,0 0-1,0 1 1,0 0 0,19 0 0,-20 2 65,17 3-464,-26-1 381,0-1-1,-1 0 0,1 1 1,0-1-1,-1 1 1,1-1-1,-1 0 0,1 1 1,-1-1-1,0 1 0,1 0 1,-1-1-1,0 1 0,0-1 1,0 1-1,-1 2 0,1 0 36,-1-1-1,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0-1 1,-1 1-1,1-1 0,-1 1 1,-3 2-1,-59 38 34,52-35-56,-25 15-635,-56 23 0,102-45 681,-1 0 0,1 1 0,0 0-1,-1 0 1,1 1 0,-1 0 0,0 0 0,0 1 0,12 8-1,-11-7-188,0 0 0,0-1 0,0 0 0,1 0 0,0-1 0,-1 0-1,1 0 1,13 1 0,38-3-6575,-31-1 1767</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8498.95">4758 1589 3314,'0'0'12194,"0"-8"-11768,0 5-444,0 5 80,-14 183 1039,1-23 533,13-185-1355,-1 2-204,1 0 0,2-1 1,0 1-1,1 0 0,7-29 1,3 12-188,1 0-1,2 0 1,1 2 0,2 0 0,37-52 0,-54 85 84,1-1 0,0 1 0,-1-1 0,1 1 0,1 0-1,-1 0 1,0 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0 0 0,0-1 0,1 1-1,7 0 1,-11 9-361,0 3 394,-1 1 0,-1-1 1,0 0-1,0 0 1,-1 0-1,-1 0 0,0 0 1,0 0-1,-1-1 0,-1 1 1,-7 13-1,-10 9 102,9-17-64,2 2 0,-12 21-1,21-34-56,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1 0-1,1 0 1,-1 0 0,1 0 0,-1 1 0,2-1 0,-1 0-1,2 9 1,-1-11 13,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,5 1 0,-3-1 11,-1 1 1,1 0 0,0 0-1,-1 0 1,0 1-1,1-1 1,-1 1-1,5 4 1,-9-6-12,1-1 1,-1 0-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 1-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,0 0-1,0-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 1,-2 1-1,-23 10 144,21-9-108,-68 29 386,23-9-521,-64 20 1,113-42-217,-7 0-8,18-18-11663</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8498.94">4758 1589 3314,'0'0'12194,"0"-8"-11768,0 5-444,0 5 80,-14 183 1039,1-23 533,13-185-1355,-1 2-204,1 0 0,2-1 1,0 1-1,1 0 0,7-29 1,3 12-188,1 0-1,2 0 1,1 2 0,2 0 0,37-52 0,-54 85 84,1-1 0,0 1 0,-1-1 0,1 1 0,1 0-1,-1 0 1,0 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0 0 0,0-1 0,1 1-1,7 0 1,-11 9-361,0 3 394,-1 1 0,-1-1 1,0 0-1,0 0 1,-1 0-1,-1 0 0,0 0 1,0 0-1,-1-1 0,-1 1 1,-7 13-1,-10 9 102,9-17-64,2 2 0,-12 21-1,21-34-56,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1 0-1,1 0 1,-1 0 0,1 0 0,-1 1 0,2-1 0,-1 0-1,2 9 1,-1-11 13,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,5 1 0,-3-1 11,-1 1 1,1 0 0,0 0-1,-1 0 1,0 1-1,1-1 1,-1 1-1,5 4 1,-9-6-12,1-1 1,-1 0-1,1 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 1-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,0 0-1,0-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1-1 1,-2 1-1,-23 10 144,21-9-108,-68 29 386,23-9-521,-64 20 1,113-42-217,-7 0-8,18-18-11663</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8814.44">5064 1702 1072,'0'0'12897,"-7"12"-12041,-2 6-644,0-1 0,1 1-1,0 1 1,2-1 0,0 1-1,1 0 1,1 1 0,-2 20-1,6-28-192,0-10-21,0 0-1,-1-1 1,1 1-1,0 0 1,1 0-1,-1 0 1,0 0-1,0-1 1,1 1-1,-1 0 1,1 0-1,1 3 1,-1-4 3,1 0 0,-1 0 1,1-1-1,0 1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1 1 0,0-1 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 0 0,2-1 0,-1 1 32,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1-1 1,-1 1 0,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,0 0-1,1-5 1,1-6-246,0-1 0,-1 1 0,-1-1 0,0-21 1,-3 35-424,-1 1 1,1-1 0,-1 0 0,1 0 0,-1 1 0,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-4 2 0</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9147.33">5302 1777 2817,'0'0'11320,"-26"21"-10600,-79 70-194,101-89-502,1 1-1,0 0 1,0 0 0,0 0 0,0 0-1,1 1 1,-1-1 0,1 1 0,0 0-1,0-1 1,0 1 0,1 0-1,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,1 1 0,-1-1 0,1 0-1,1 7 1,-1 1-31,0-11-2,0 1 1,0-1-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,1 1-1,-1-1 0,0 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0-1 0,-1 1 1,1 0-1,0 0 0,0-1 1,0 1-1,0 0 0,0-1 1,2 2-1,0-1 5,0 0 0,1-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,0 0 0,1 0 0,4-1 0,-1 0 52,0 0-1,-1 0 1,1-1-1,-1 0 1,0 0-1,1 0 1,-1-1 0,0 0-1,8-6 1,-8 3-14,-1 0 0,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 0,-1-1 1,0 1-1,0-1 1,-1 0-1,0 0 0,0 0 1,-1 0-1,0 0 1,0 0-1,-1 0 0,0 0 1,0-1-1,-1 1 1,0 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,-1 1-1,-1-1 0,-6-12 1,7 16-303,-6-14-865,6 6-3010,3 7-430</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9678.27">5431 1531 4978,'0'0'10530,"0"17"-10143,0 23 134,-2 1-1,-2-1 0,-11 48 0,-7-3-53,-17 60-29,35-166 709,4-15-1091,3 21-50,1 0 0,0 0 0,2 1 0,-1-1 1,2 1-1,9-15 0,-12 21-20,0 0 1,1 1 0,0 0-1,0 0 1,1 1 0,0-1-1,0 1 1,1 1 0,-1-1-1,1 1 1,1 0 0,12-6-1,-18 10-2,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,0 0 0,1 0 0,-1-1 0,0 1 1,0 1-1,0-1 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,2 3 0,-2-1-19,0-1-1,-1 1 1,0 0-1,1 0 1,-1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,-1 5-1,0-4 24,-1 0 0,1-1 1,0 1-1,-1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-6 3 0,-61 36-142,46-30 43,37-3 119,0-1 1,29 12-1,-37-17 28,70 44 749,-74-45-729,-1-1-158,-16-1-5772,-8 0-1148</inkml:trace>
@@ -5382,7 +5452,7 @@
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="14" t="s">
         <v>31</v>
       </c>
       <c r="H27" t="s">
@@ -5396,7 +5466,7 @@
       <c r="B28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="14"/>
       <c r="H28" t="s">
         <v>26</v>
       </c>
@@ -5426,88 +5496,88 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="4" customFormat="1"/>
+    <row r="43" spans="2:2" s="3" customFormat="1"/>
     <row r="45" spans="2:2" ht="17.649999999999999">
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="6"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="17.649999999999999">
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="6"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="17.649999999999999">
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="6"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="2:2">
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="7" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="17.649999999999999">
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5517,241 +5587,241 @@
       </c>
     </row>
     <row r="71" spans="2:2" ht="15.75">
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="6"/>
+      <c r="B72" s="5"/>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="7" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="78" spans="2:2" ht="15.75">
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="6"/>
+      <c r="B79" s="5"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="7" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="7" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="7" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="15.75">
-      <c r="B85" s="9" t="s">
+      <c r="B85" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="86" spans="2:2">
-      <c r="B86" s="6"/>
+      <c r="B86" s="5"/>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="7" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="89" spans="2:2">
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="7" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="15.75">
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="6"/>
+      <c r="B93" s="5"/>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="7" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="7" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="96" spans="2:2">
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="7" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="97" spans="2:2">
-      <c r="B97" s="8" t="s">
+      <c r="B97" s="7" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="15.75">
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="6"/>
+      <c r="B100" s="5"/>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="8" t="s">
+      <c r="B101" s="7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="7" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="103" spans="2:2">
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="7" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="104" spans="2:2">
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="7" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="106" spans="2:2" ht="15.75">
-      <c r="B106" s="9" t="s">
+      <c r="B106" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="6"/>
+      <c r="B107" s="5"/>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="8" t="s">
+      <c r="B108" s="7" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="8" t="s">
+      <c r="B109" s="7" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="8" t="s">
+      <c r="B110" s="7" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="8" t="s">
+      <c r="B111" s="7" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="15.75">
-      <c r="B113" s="9" t="s">
+      <c r="B113" s="8" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="6"/>
+      <c r="B114" s="5"/>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="8" t="s">
+      <c r="B115" s="7" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="8" t="s">
+      <c r="B116" s="7" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="8" t="s">
+      <c r="B117" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="8" t="s">
+      <c r="B118" s="7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="17.649999999999999">
-      <c r="B121" s="5" t="s">
+      <c r="B121" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="6"/>
+      <c r="B122" s="5"/>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="8" t="s">
+      <c r="B123" s="7" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="124" spans="2:2">
-      <c r="B124" s="8" t="s">
+      <c r="B124" s="7" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" s="8" t="s">
+      <c r="B125" s="7" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="8" t="s">
+      <c r="B126" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="8" t="s">
+      <c r="B127" s="7" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="8" t="s">
+      <c r="B128" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="8" t="s">
+      <c r="B129" s="7" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5761,156 +5831,156 @@
       </c>
     </row>
     <row r="133" spans="2:2" ht="17.649999999999999">
-      <c r="B133" s="5" t="s">
+      <c r="B133" s="4" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="6"/>
+      <c r="B134" s="5"/>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="7" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="8" t="s">
+      <c r="B136" s="7" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="8" t="s">
+      <c r="B137" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="138" spans="2:2">
-      <c r="B138" s="8" t="s">
+      <c r="B138" s="7" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="17.649999999999999">
-      <c r="B140" s="5" t="s">
+      <c r="B140" s="4" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="6"/>
+      <c r="B141" s="5"/>
     </row>
     <row r="142" spans="2:2">
-      <c r="B142" s="8" t="s">
+      <c r="B142" s="7" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="8" t="s">
+      <c r="B143" s="7" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="8" t="s">
+      <c r="B144" s="7" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="8" t="s">
+      <c r="B145" s="7" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="17.649999999999999">
-      <c r="B147" s="5" t="s">
+      <c r="B147" s="4" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="6"/>
+      <c r="B148" s="5"/>
     </row>
     <row r="149" spans="2:2">
-      <c r="B149" s="8" t="s">
+      <c r="B149" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="150" spans="2:2">
-      <c r="B150" s="8" t="s">
+      <c r="B150" s="7" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="151" spans="2:2">
-      <c r="B151" s="8" t="s">
+      <c r="B151" s="7" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="152" spans="2:2">
-      <c r="B152" s="8" t="s">
+      <c r="B152" s="7" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="154" spans="2:2" ht="17.649999999999999">
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="4" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="155" spans="2:2">
-      <c r="B155" s="6"/>
+      <c r="B155" s="5"/>
     </row>
     <row r="156" spans="2:2">
-      <c r="B156" s="8" t="s">
+      <c r="B156" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="157" spans="2:2">
-      <c r="B157" s="8" t="s">
+      <c r="B157" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="158" spans="2:2">
-      <c r="B158" s="8" t="s">
+      <c r="B158" s="7" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="159" spans="2:2">
-      <c r="B159" s="8" t="s">
+      <c r="B159" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="163" spans="2:2" ht="17.649999999999999">
-      <c r="B163" s="5" t="s">
+      <c r="B163" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="164" spans="2:2">
-      <c r="B164" s="6"/>
+      <c r="B164" s="5"/>
     </row>
     <row r="165" spans="2:2">
-      <c r="B165" s="8" t="s">
+      <c r="B165" s="7" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="166" spans="2:2">
-      <c r="B166" s="6"/>
+      <c r="B166" s="5"/>
     </row>
     <row r="167" spans="2:2">
-      <c r="B167" s="8" t="s">
+      <c r="B167" s="7" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="168" spans="2:2">
-      <c r="B168" s="6"/>
+      <c r="B168" s="5"/>
     </row>
     <row r="169" spans="2:2">
-      <c r="B169" s="8" t="s">
+      <c r="B169" s="7" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="170" spans="2:2">
-      <c r="B170" s="6"/>
+      <c r="B170" s="5"/>
     </row>
     <row r="171" spans="2:2">
-      <c r="B171" s="8" t="s">
+      <c r="B171" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="175" spans="2:2" ht="17.649999999999999">
-      <c r="B175" s="5" t="s">
+      <c r="B175" s="4" t="s">
         <v>177</v>
       </c>
     </row>
@@ -5920,499 +5990,499 @@
       </c>
     </row>
     <row r="178" spans="2:2">
-      <c r="B178" s="6"/>
+      <c r="B178" s="5"/>
     </row>
     <row r="179" spans="2:2">
-      <c r="B179" s="8" t="s">
+      <c r="B179" s="7" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="180" spans="2:2">
-      <c r="B180" s="8" t="s">
+      <c r="B180" s="7" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="181" spans="2:2">
-      <c r="B181" s="8" t="s">
+      <c r="B181" s="7" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="182" spans="2:2">
-      <c r="B182" s="8" t="s">
+      <c r="B182" s="7" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="211" spans="2:2">
-      <c r="B211" s="7" t="s">
+      <c r="B211" s="6" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="17.649999999999999">
-      <c r="B213" s="5" t="s">
+      <c r="B213" s="4" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="214" spans="2:2">
-      <c r="B214" s="6"/>
+      <c r="B214" s="5"/>
     </row>
     <row r="215" spans="2:2">
-      <c r="B215" s="8" t="s">
+      <c r="B215" s="7" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="216" spans="2:2">
-      <c r="B216" s="8" t="s">
+      <c r="B216" s="7" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="17.649999999999999">
-      <c r="B218" s="5" t="s">
+      <c r="B218" s="4" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="219" spans="2:2">
-      <c r="B219" s="6"/>
+      <c r="B219" s="5"/>
     </row>
     <row r="220" spans="2:2">
-      <c r="B220" s="8" t="s">
+      <c r="B220" s="7" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="221" spans="2:2">
-      <c r="B221" s="6"/>
+      <c r="B221" s="5"/>
     </row>
     <row r="222" spans="2:2">
-      <c r="B222" s="8" t="s">
+      <c r="B222" s="7" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="223" spans="2:2">
-      <c r="B223" s="6"/>
+      <c r="B223" s="5"/>
     </row>
     <row r="224" spans="2:2">
-      <c r="B224" s="8" t="s">
+      <c r="B224" s="7" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="225" spans="2:2">
-      <c r="B225" s="6"/>
+      <c r="B225" s="5"/>
     </row>
     <row r="226" spans="2:2">
-      <c r="B226" s="8" t="s">
+      <c r="B226" s="7" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="228" spans="2:2" ht="17.649999999999999">
-      <c r="B228" s="5" t="s">
+      <c r="B228" s="4" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="229" spans="2:2">
-      <c r="B229" s="6"/>
+      <c r="B229" s="5"/>
     </row>
     <row r="230" spans="2:2">
-      <c r="B230" s="8" t="s">
+      <c r="B230" s="7" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="232" spans="2:2" ht="17.649999999999999">
-      <c r="B232" s="5" t="s">
+      <c r="B232" s="4" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="234" spans="2:2">
-      <c r="B234" s="7" t="s">
+      <c r="B234" s="6" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="236" spans="2:2">
-      <c r="B236" s="7" t="s">
+      <c r="B236" s="6" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="237" spans="2:2">
-      <c r="B237" s="6"/>
+      <c r="B237" s="5"/>
     </row>
     <row r="238" spans="2:2">
-      <c r="B238" s="8" t="s">
+      <c r="B238" s="7" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="239" spans="2:2">
-      <c r="B239" s="8" t="s">
+      <c r="B239" s="7" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="240" spans="2:2">
-      <c r="B240" s="8" t="s">
+      <c r="B240" s="7" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="242" spans="2:2">
-      <c r="B242" s="7" t="s">
+      <c r="B242" s="6" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="243" spans="2:2">
-      <c r="B243" s="6"/>
+      <c r="B243" s="5"/>
     </row>
     <row r="244" spans="2:2">
-      <c r="B244" s="8" t="s">
+      <c r="B244" s="7" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="245" spans="2:2">
-      <c r="B245" s="8" t="s">
+      <c r="B245" s="7" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="246" spans="2:2">
-      <c r="B246" s="8" t="s">
+      <c r="B246" s="7" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="248" spans="2:2">
-      <c r="B248" s="7" t="s">
+      <c r="B248" s="6" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="249" spans="2:2">
-      <c r="B249" s="6"/>
+      <c r="B249" s="5"/>
     </row>
     <row r="250" spans="2:2">
-      <c r="B250" s="8" t="s">
+      <c r="B250" s="7" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="251" spans="2:2">
-      <c r="B251" s="8" t="s">
+      <c r="B251" s="7" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="252" spans="2:2">
-      <c r="B252" s="8" t="s">
+      <c r="B252" s="7" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="254" spans="2:2">
-      <c r="B254" s="7" t="s">
+      <c r="B254" s="6" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="255" spans="2:2">
-      <c r="B255" s="6"/>
+      <c r="B255" s="5"/>
     </row>
     <row r="256" spans="2:2">
-      <c r="B256" s="8" t="s">
+      <c r="B256" s="7" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="257" spans="2:2">
-      <c r="B257" s="8" t="s">
+      <c r="B257" s="7" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="258" spans="2:2">
-      <c r="B258" s="8" t="s">
+      <c r="B258" s="7" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="260" spans="2:2">
-      <c r="B260" s="7" t="s">
+      <c r="B260" s="6" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="261" spans="2:2">
-      <c r="B261" s="6"/>
+      <c r="B261" s="5"/>
     </row>
     <row r="262" spans="2:2">
-      <c r="B262" s="8" t="s">
+      <c r="B262" s="7" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="263" spans="2:2">
-      <c r="B263" s="8" t="s">
+      <c r="B263" s="7" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="264" spans="2:2">
-      <c r="B264" s="8" t="s">
+      <c r="B264" s="7" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="266" spans="2:2">
-      <c r="B266" s="7" t="s">
+      <c r="B266" s="6" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="267" spans="2:2">
-      <c r="B267" s="6"/>
+      <c r="B267" s="5"/>
     </row>
     <row r="268" spans="2:2">
-      <c r="B268" s="8" t="s">
+      <c r="B268" s="7" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="269" spans="2:2">
-      <c r="B269" s="8" t="s">
+      <c r="B269" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="270" spans="2:2">
-      <c r="B270" s="8" t="s">
+      <c r="B270" s="7" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="272" spans="2:2">
-      <c r="B272" s="7" t="s">
+      <c r="B272" s="6" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="273" spans="2:2">
-      <c r="B273" s="6"/>
+      <c r="B273" s="5"/>
     </row>
     <row r="274" spans="2:2">
-      <c r="B274" s="8" t="s">
+      <c r="B274" s="7" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="275" spans="2:2">
-      <c r="B275" s="8" t="s">
+      <c r="B275" s="7" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="276" spans="2:2">
-      <c r="B276" s="8" t="s">
+      <c r="B276" s="7" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="278" spans="2:2">
-      <c r="B278" s="7" t="s">
+      <c r="B278" s="6" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="279" spans="2:2">
-      <c r="B279" s="6"/>
+      <c r="B279" s="5"/>
     </row>
     <row r="280" spans="2:2">
-      <c r="B280" s="8" t="s">
+      <c r="B280" s="7" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="281" spans="2:2">
-      <c r="B281" s="8" t="s">
+      <c r="B281" s="7" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="282" spans="2:2">
-      <c r="B282" s="8" t="s">
+      <c r="B282" s="7" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="284" spans="2:2">
-      <c r="B284" s="7" t="s">
+      <c r="B284" s="6" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="285" spans="2:2">
-      <c r="B285" s="6"/>
+      <c r="B285" s="5"/>
     </row>
     <row r="286" spans="2:2">
-      <c r="B286" s="8" t="s">
+      <c r="B286" s="7" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="287" spans="2:2">
-      <c r="B287" s="8" t="s">
+      <c r="B287" s="7" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="288" spans="2:2">
-      <c r="B288" s="8" t="s">
+      <c r="B288" s="7" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="290" spans="2:2">
-      <c r="B290" s="7" t="s">
+      <c r="B290" s="6" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="291" spans="2:2">
-      <c r="B291" s="6"/>
+      <c r="B291" s="5"/>
     </row>
     <row r="292" spans="2:2">
-      <c r="B292" s="8" t="s">
+      <c r="B292" s="7" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="293" spans="2:2">
-      <c r="B293" s="8" t="s">
+      <c r="B293" s="7" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="294" spans="2:2">
-      <c r="B294" s="8" t="s">
+      <c r="B294" s="7" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="296" spans="2:2">
-      <c r="B296" s="7" t="s">
+      <c r="B296" s="6" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="297" spans="2:2">
-      <c r="B297" s="6"/>
+      <c r="B297" s="5"/>
     </row>
     <row r="298" spans="2:2">
-      <c r="B298" s="8" t="s">
+      <c r="B298" s="7" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="299" spans="2:2">
-      <c r="B299" s="8" t="s">
+      <c r="B299" s="7" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="300" spans="2:2">
-      <c r="B300" s="8" t="s">
+      <c r="B300" s="7" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="302" spans="2:2">
-      <c r="B302" s="7" t="s">
+      <c r="B302" s="6" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="303" spans="2:2">
-      <c r="B303" s="6"/>
+      <c r="B303" s="5"/>
     </row>
     <row r="304" spans="2:2">
-      <c r="B304" s="8" t="s">
+      <c r="B304" s="7" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="305" spans="2:2">
-      <c r="B305" s="8" t="s">
+      <c r="B305" s="7" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="306" spans="2:2">
-      <c r="B306" s="8" t="s">
+      <c r="B306" s="7" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="308" spans="2:2">
-      <c r="B308" s="7" t="s">
+      <c r="B308" s="6" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="309" spans="2:2">
-      <c r="B309" s="6"/>
+      <c r="B309" s="5"/>
     </row>
     <row r="310" spans="2:2">
-      <c r="B310" s="8" t="s">
+      <c r="B310" s="7" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="311" spans="2:2">
-      <c r="B311" s="8" t="s">
+      <c r="B311" s="7" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="312" spans="2:2">
-      <c r="B312" s="8" t="s">
+      <c r="B312" s="7" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="314" spans="2:2">
-      <c r="B314" s="7" t="s">
+      <c r="B314" s="6" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="315" spans="2:2">
-      <c r="B315" s="6"/>
+      <c r="B315" s="5"/>
     </row>
     <row r="316" spans="2:2">
-      <c r="B316" s="8" t="s">
+      <c r="B316" s="7" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="317" spans="2:2">
-      <c r="B317" s="8" t="s">
+      <c r="B317" s="7" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="318" spans="2:2">
-      <c r="B318" s="8" t="s">
+      <c r="B318" s="7" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="320" spans="2:2">
-      <c r="B320" s="7" t="s">
+      <c r="B320" s="6" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="321" spans="2:2">
-      <c r="B321" s="6"/>
+      <c r="B321" s="5"/>
     </row>
     <row r="322" spans="2:2">
-      <c r="B322" s="8" t="s">
+      <c r="B322" s="7" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="323" spans="2:2">
-      <c r="B323" s="8" t="s">
+      <c r="B323" s="7" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="324" spans="2:2">
-      <c r="B324" s="8" t="s">
+      <c r="B324" s="7" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="326" spans="2:2">
-      <c r="B326" s="7" t="s">
+      <c r="B326" s="6" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="327" spans="2:2">
-      <c r="B327" s="6"/>
+      <c r="B327" s="5"/>
     </row>
     <row r="328" spans="2:2">
-      <c r="B328" s="8" t="s">
+      <c r="B328" s="7" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="329" spans="2:2">
-      <c r="B329" s="8" t="s">
+      <c r="B329" s="7" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="330" spans="2:2">
-      <c r="B330" s="8" t="s">
+      <c r="B330" s="7" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="332" spans="2:2">
-      <c r="B332" s="7" t="s">
+      <c r="B332" s="6" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="333" spans="2:2">
-      <c r="B333" s="6"/>
+      <c r="B333" s="5"/>
     </row>
     <row r="334" spans="2:2">
-      <c r="B334" s="8" t="s">
+      <c r="B334" s="7" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="335" spans="2:2">
-      <c r="B335" s="8" t="s">
+      <c r="B335" s="7" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="336" spans="2:2">
-      <c r="B336" s="8" t="s">
+      <c r="B336" s="7" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6448,10 +6518,10 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F3" t="s">
@@ -6462,10 +6532,10 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F4" t="s">
@@ -6479,7 +6549,7 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H5" t="s">
@@ -6493,7 +6563,7 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>57</v>
       </c>
       <c r="I6" t="s">
@@ -6504,7 +6574,7 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>58</v>
       </c>
       <c r="I7" t="s">
@@ -6557,12 +6627,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:7" s="4" customFormat="1"/>
+    <row r="18" spans="2:7" s="3" customFormat="1"/>
     <row r="20" spans="2:7">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" t="s">
@@ -6648,9 +6718,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:7" s="4" customFormat="1"/>
+    <row r="29" spans="2:7" s="3" customFormat="1"/>
     <row r="31" spans="2:7" ht="21">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>71</v>
       </c>
       <c r="D31" t="s">
@@ -6658,29 +6728,29 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="21">
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="21">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="21">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="21">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="2:4" s="4" customFormat="1"/>
+    <row r="37" spans="2:4" s="3" customFormat="1"/>
     <row r="39" spans="2:4">
       <c r="B39" t="s">
         <v>77</v>
@@ -6757,8 +6827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="C212" sqref="C212"/>
+    <sheetView topLeftCell="A190" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6768,41 +6838,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="2:10">
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="5" spans="2:10" s="4" customFormat="1">
-      <c r="B5" s="4" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="5" spans="2:10" s="3" customFormat="1">
+      <c r="B5" s="3" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6851,7 +6921,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="2:5" s="4" customFormat="1"/>
+    <row r="19" spans="2:5" s="3" customFormat="1"/>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
         <v>272</v>
@@ -6974,7 +7044,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="4" customFormat="1"/>
+    <row r="39" spans="2:5" s="3" customFormat="1"/>
     <row r="41" spans="2:5">
       <c r="B41" t="s">
         <v>300</v>
@@ -6997,7 +7067,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="44" spans="2:5" s="4" customFormat="1"/>
+    <row r="44" spans="2:5" s="3" customFormat="1"/>
     <row r="46" spans="2:5">
       <c r="C46" t="s">
         <v>305</v>
@@ -7008,7 +7078,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="50" spans="2:3" s="4" customFormat="1"/>
+    <row r="50" spans="2:3" s="3" customFormat="1"/>
     <row r="52" spans="2:3">
       <c r="B52" t="s">
         <v>307</v>
@@ -7025,194 +7095,194 @@
       </c>
     </row>
     <row r="57" spans="2:3">
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="17.649999999999999">
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="B60" s="6"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="2:3">
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="62" spans="2:3">
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="7" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="63" spans="2:3">
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="7" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="64" spans="2:3">
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="65" spans="2:4">
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="7" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="66" spans="2:4">
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="7" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="68" spans="2:4" ht="17.649999999999999">
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="4" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="69" spans="2:4">
-      <c r="B69" s="6"/>
+      <c r="B69" s="5"/>
     </row>
     <row r="70" spans="2:4">
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="7" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="71" spans="2:4">
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="7" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="72" spans="2:4">
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="7" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="73" spans="2:4">
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="7" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="74" spans="2:4">
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="7" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="75" spans="2:4">
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="7" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="77" spans="2:4" ht="17.649999999999999">
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="79" spans="2:4">
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" s="10" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="80" spans="2:4" ht="28.5">
-      <c r="B80" s="15" t="s">
+    <row r="80" spans="2:4">
+      <c r="B80" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="12" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="81" spans="2:4" ht="42.75">
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C81" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="11" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="82" spans="2:4" ht="42.75">
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="11" t="s">
         <v>334</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="D82" s="15" t="s">
+      <c r="D82" s="11" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="83" spans="2:4" ht="42.75">
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="C83" s="15" t="s">
+      <c r="C83" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D83" s="11" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="84" spans="2:4" ht="28.5">
-      <c r="B84" s="15" t="s">
+      <c r="B84" s="11" t="s">
         <v>340</v>
       </c>
-      <c r="C84" s="15" t="s">
+      <c r="C84" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="D84" s="11" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="28.5">
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="C85" s="15" t="s">
+      <c r="C85" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="D85" s="15" t="s">
+      <c r="D85" s="11" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="86" spans="2:4" ht="28.5">
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="D86" s="15" t="s">
+      <c r="D86" s="11" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="88" spans="2:4" ht="17.649999999999999">
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="4" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="89" spans="2:4">
-      <c r="B89" s="6"/>
+      <c r="B89" s="5"/>
     </row>
     <row r="90" spans="2:4">
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="7" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="91" spans="2:4">
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="7" t="s">
         <v>351</v>
       </c>
     </row>
@@ -7221,7 +7291,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="95" spans="2:4" s="4" customFormat="1"/>
+    <row r="95" spans="2:4" s="3" customFormat="1"/>
     <row r="97" spans="2:3">
       <c r="B97" t="s">
         <v>353</v>
@@ -7263,7 +7333,7 @@
       </c>
     </row>
     <row r="130" spans="2:3">
-      <c r="B130" s="17">
+      <c r="B130" s="13">
         <f ca="1">TODAY()</f>
         <v>45605</v>
       </c>
@@ -7288,7 +7358,7 @@
       <c r="C151" t="s">
         <v>363</v>
       </c>
-      <c r="D151" s="4"/>
+      <c r="D151" s="3"/>
     </row>
     <row r="153" spans="3:4">
       <c r="C153" t="s">
@@ -7299,7 +7369,7 @@
       <c r="C154" t="s">
         <v>365</v>
       </c>
-      <c r="D154" s="4" t="s">
+      <c r="D154" s="3" t="s">
         <v>368</v>
       </c>
     </row>
@@ -7333,7 +7403,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="195" spans="2:3" s="4" customFormat="1"/>
+    <row r="195" spans="2:3" s="3" customFormat="1"/>
     <row r="196" spans="2:3">
       <c r="C196" t="s">
         <v>375</v>
@@ -7364,8 +7434,8 @@
         <v>374</v>
       </c>
     </row>
-    <row r="207" spans="2:3" s="4" customFormat="1">
-      <c r="B207" s="4" t="s">
+    <row r="207" spans="2:3" s="3" customFormat="1">
+      <c r="B207" s="3" t="s">
         <v>374</v>
       </c>
     </row>
@@ -7381,4 +7451,147 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CBD97B-9891-44B9-9DA8-3C71B6EDF689}">
+  <dimension ref="B2:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>380</v>
+      </c>
+      <c r="F3" t="s">
+        <v>391</v>
+      </c>
+      <c r="G3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F4" t="s">
+        <v>392</v>
+      </c>
+      <c r="G4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F5" t="s">
+        <v>393</v>
+      </c>
+      <c r="G5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>382</v>
+      </c>
+      <c r="F6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G6" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
+        <v>383</v>
+      </c>
+      <c r="F7" t="s">
+        <v>400</v>
+      </c>
+      <c r="G7" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="16.5">
+      <c r="B14" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="16.5">
+      <c r="B15" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="16.5">
+      <c r="B16" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="16.5">
+      <c r="B17" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="16.5">
+      <c r="B18" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="16.5">
+      <c r="B19" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="16.5">
+      <c r="B20" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>